<commit_message>
thêm giang vien trong file account/lecturer.xlsx + xu li truong hop trung ten
</commit_message>
<xml_diff>
--- a/account/lecturer.xlsx
+++ b/account/lecturer.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\Tiểu luận - NMLT\account\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\python\TL\TLGiang\account\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C580E79B-266A-49F3-ADBD-C8DF1245E6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{0DCF8658-FBD3-4355-B155-FC83ABA0D826}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Mật khẩu</t>
   </si>
@@ -54,9 +53,6 @@
     <t>Nguyễn Văn Z</t>
   </si>
   <si>
-    <t>Ngô Văn Q</t>
-  </si>
-  <si>
     <t>Trần Văn Q</t>
   </si>
   <si>
@@ -76,12 +72,45 @@
   </si>
   <si>
     <t>GIS_DC</t>
+  </si>
+  <si>
+    <t>Đặng Văn Q</t>
+  </si>
+  <si>
+    <t>Mã giảng viên</t>
+  </si>
+  <si>
+    <t>n01</t>
+  </si>
+  <si>
+    <t>n02</t>
+  </si>
+  <si>
+    <t>n03</t>
+  </si>
+  <si>
+    <t>k01</t>
+  </si>
+  <si>
+    <t>k02</t>
+  </si>
+  <si>
+    <t>gp01</t>
+  </si>
+  <si>
+    <t>gp02</t>
+  </si>
+  <si>
+    <t>gi01</t>
+  </si>
+  <si>
+    <t>gi02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,12 +120,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,8 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,19 +469,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25014AA-F72D-46DC-91FD-E2A8BF68B3D4}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -448,82 +492,134 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C7" s="2">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C8" s="2">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>123</v>
+      <c r="C9">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>123</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>